<commit_message>
aded gerber files, pcd design finished
</commit_message>
<xml_diff>
--- a/BOM/BOM PM9080.xlsx
+++ b/BOM/BOM PM9080.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\fluke_pm9080\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD10B71-3B98-4C1A-BBAC-71F7F5A0177A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51948A4-C80D-42A6-AA50-37645E660FD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17130" yWindow="1170" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{3C56C210-DCD0-4B76-B854-73BBFDBB2958}"/>
+    <workbookView xWindow="7200" yWindow="1170" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{3C56C210-DCD0-4B76-B854-73BBFDBB2958}"/>
   </bookViews>
   <sheets>
     <sheet name="USB" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
   <si>
     <t>Farnell</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>LM393ADR</t>
+  </si>
+  <si>
+    <t>RJ11</t>
   </si>
 </sst>
 </file>
@@ -479,7 +482,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,10 +725,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B797A86F-6142-4D79-8995-3E4C349A6E7D}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +874,7 @@
         <v>0.17599999999999999</v>
       </c>
       <c r="E7">
-        <f t="shared" ref="E7:E13" si="1">C7*D7</f>
+        <f t="shared" ref="E7:E14" si="1">C7*D7</f>
         <v>0.17599999999999999</v>
       </c>
       <c r="F7" t="s">
@@ -943,7 +946,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>1497880</v>
+        <v>2709041</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
@@ -952,69 +955,90 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <v>0.96499999999999997</v>
+        <v>0.8</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>0.96499999999999997</v>
+        <v>0.8</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>1497871</v>
+        <v>1497880</v>
       </c>
       <c r="B12" t="s">
         <v>0</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0.96499999999999997</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.96499999999999997</v>
       </c>
       <c r="F12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>1497864</v>
+        <v>1497871</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
       </c>
       <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>1.04</v>
+        <v>0</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>1497864</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
         <v>1.04</v>
       </c>
-      <c r="F13" t="s">
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>1.04</v>
+      </c>
+      <c r="F14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
         <v>10</v>
       </c>
-      <c r="E15">
-        <f>SUM(E2:E12)</f>
-        <v>6.3743999999999996</v>
+      <c r="E16">
+        <f>SUM(E2:E13)</f>
+        <v>7.1743999999999994</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A11" r:id="rId1" display="https://be.farnell.com/tt-electronics-optek-technology/op506a/phototransistor-plastic-t-1/dp/1497880?scope=partnumberlookahead&amp;ost=1497880&amp;searchref=searchlookahead&amp;exaMfpn=true&amp;ddkey=https%3Anl-BE%2FElement14_Belgium%2Fw%2Fsearch" xr:uid="{5C79944D-9CBD-46AE-B9EC-73D3B19F40A6}"/>
-    <hyperlink ref="A13" r:id="rId2" display="https://be.farnell.com/tt-electronics-optek-technology/op165a/infrared-emitter-935nm-t-1/dp/1497864" xr:uid="{8CB128B6-63A4-4656-958B-188823561009}"/>
-    <hyperlink ref="A12" r:id="rId3" display="https://be.farnell.com/tt-electronics-optek-technology/op265a/infrared-emitter-890nm-t-1/dp/1497871?scope=partnumberlookahead&amp;ost=OP265A&amp;searchref=searchlookahead&amp;exaMfpn=true" xr:uid="{D5D2B4BB-5FF0-4EBA-9E36-6FCA41663247}"/>
+    <hyperlink ref="A12" r:id="rId1" display="https://be.farnell.com/tt-electronics-optek-technology/op506a/phototransistor-plastic-t-1/dp/1497880?scope=partnumberlookahead&amp;ost=1497880&amp;searchref=searchlookahead&amp;exaMfpn=true&amp;ddkey=https%3Anl-BE%2FElement14_Belgium%2Fw%2Fsearch" xr:uid="{5C79944D-9CBD-46AE-B9EC-73D3B19F40A6}"/>
+    <hyperlink ref="A14" r:id="rId2" display="https://be.farnell.com/tt-electronics-optek-technology/op165a/infrared-emitter-935nm-t-1/dp/1497864" xr:uid="{8CB128B6-63A4-4656-958B-188823561009}"/>
+    <hyperlink ref="A13" r:id="rId3" display="https://be.farnell.com/tt-electronics-optek-technology/op265a/infrared-emitter-890nm-t-1/dp/1497871?scope=partnumberlookahead&amp;ost=OP265A&amp;searchref=searchlookahead&amp;exaMfpn=true" xr:uid="{D5D2B4BB-5FF0-4EBA-9E36-6FCA41663247}"/>
     <hyperlink ref="A3" r:id="rId4" display="https://be.farnell.com/texas-instruments/lm393adr/comparator-dual-smd-soic8-393/dp/3118467?st=lm393" xr:uid="{54EABD9C-34BF-4513-BD93-B8A56DEA01B5}"/>
     <hyperlink ref="A10" r:id="rId5" display="https://be.farnell.com/amp-te-connectivity/5747844-6/socket-d-9way/dp/1338746?st=db9" xr:uid="{4EA5A972-C971-463E-AB45-98D229CEBE1D}"/>
     <hyperlink ref="A5" r:id="rId6" display="https://be.farnell.com/vishay/crcw12065k60fkea/res-5k6-1-0-25w-1206-thick-film/dp/2139489" xr:uid="{7C74B19C-67DB-450B-A4D3-6894C12ED3DD}"/>
@@ -1023,8 +1047,9 @@
     <hyperlink ref="A8" r:id="rId9" display="https://be.farnell.com/diodes-inc/1n4148wq-7-f/diode-small-signal-100v-0-3a-sod/dp/3127171?st=1n4148" xr:uid="{6D71A9AC-9406-4906-88A0-0B32CA7AF47D}"/>
     <hyperlink ref="A9" r:id="rId10" display="https://be.farnell.com/multicomp/mcvvt025m101ea6l/cap-100-f-25v-smd/dp/2611370" xr:uid="{AD23CC01-269A-458B-9449-AC73A9995385}"/>
     <hyperlink ref="A4" r:id="rId11" display="https://be.farnell.com/bourns/3313j-1-473e/trimmer-pot-47kohm-20-1turn-smd/dp/2329337" xr:uid="{96171874-590D-4BB4-A3D0-066839DA2199}"/>
+    <hyperlink ref="A11" r:id="rId12" display="https://be.farnell.com/amphenol-icc-commercial-products/rje0166001/connector-unshld-rj11-jack-6p6c/dp/2709041?st=rj11" xr:uid="{F8E98F99-A28B-4390-AB1C-083A9268AC41}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>